<commit_message>
Change name of excel
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kean_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kean_\Documents\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0ACE23-0AC8-4855-98A3-4E692BE61822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D66F54-8F29-422C-A78B-2CD760CAB3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7D62A8B1-2462-4A04-8D93-B31AB8D66450}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
   <si>
-    <t>Review journaal</t>
-  </si>
-  <si>
     <t>Titel te reviewen LCA</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>De nieuwe EPD zal hoogstwaarschijnlijk later dit jaar (conform PCR 2.0) uitkomen. Echter voor dit rapport wordt deze EPD die conform PCR 1.0 is opgesteld worden toegepast. Dit is dus de meest representatieve EPD voor Lynpave voor een mengsel uit productiejaar 2019.</t>
+  </si>
+  <si>
+    <t>Blahblahabl</t>
   </si>
 </sst>
 </file>
@@ -964,7 +964,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -981,7 +981,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1007,55 +1007,55 @@
     </row>
     <row r="6" spans="1:8" ht="56.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
       <c r="D7" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:8" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
@@ -1066,22 +1066,22 @@
     <row r="11" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.35">
@@ -1089,13 +1089,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
@@ -1105,13 +1105,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D14" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="6"/>
@@ -1121,13 +1121,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="18"/>
@@ -1137,13 +1137,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="D16" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="6"/>
@@ -1155,13 +1155,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>86</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
@@ -1171,13 +1171,13 @@
         <v>6</v>
       </c>
       <c r="B18" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>84</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="18"/>
@@ -1497,61 +1497,61 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
       </c>
       <c r="E8" s="31">
         <v>0.94</v>
@@ -1559,71 +1559,71 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>43</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>45</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>46</v>
-      </c>
-      <c r="I14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="31">
         <v>0.93964676000000003</v>
@@ -1649,10 +1649,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="30">
         <v>1.6850949000000001E-6</v>
@@ -1678,10 +1678,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>1.7662901000000002E-2</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>0.18819869</v>
@@ -1736,10 +1736,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="30">
         <v>2.079476E-5</v>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20">
         <v>2.5742292E-2</v>
@@ -1794,10 +1794,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>0.21099454000000001</v>
@@ -1823,10 +1823,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22">
         <v>0.17703509000000001</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>0.21353219000000001</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>1.3658225E-2</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>9.1336155000000002E-2</v>
@@ -1939,10 +1939,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>1.4641921E-3</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1997,10 +1997,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2055,10 +2055,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2084,10 +2084,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2113,10 +2113,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2200,10 +2200,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2229,10 +2229,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2258,10 +2258,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2287,10 +2287,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2316,10 +2316,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2345,10 +2345,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2374,10 +2374,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2403,10 +2403,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2432,10 +2432,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44">
         <v>0</v>

</xml_diff>